<commit_message>
Update backup data files and code changes
</commit_message>
<xml_diff>
--- a/assets/v5/Financial_Model_TEMPLATE_ZERO_USD_thousands_GAAP.xlsx
+++ b/assets/v5/Financial_Model_TEMPLATE_ZERO_USD_thousands_GAAP.xlsx
@@ -1859,6 +1859,7 @@
   <cols>
     <col width="41.1796875" customWidth="1" style="14" min="1" max="1"/>
     <col width="13.08984375" customWidth="1" style="14" min="2" max="9"/>
+    <col hidden="1" width="13" customWidth="1" min="5" max="5"/>
     <col width="2.36328125" customWidth="1" style="14" min="10" max="10"/>
     <col width="34.54296875" customWidth="1" style="14" min="11" max="11"/>
     <col width="9.08984375" customWidth="1" style="14" min="12" max="16384"/>
@@ -1889,6 +1890,9 @@
       <c r="D2" s="91" t="n">
         <v>2025</v>
       </c>
+      <c r="E2" t="n">
+        <v>2022</v>
+      </c>
     </row>
     <row r="3" ht="14.5" customFormat="1" customHeight="1" s="58">
       <c r="A3" s="59" t="inlineStr">
@@ -2973,8 +2977,9 @@
           <t>Retained Earnings</t>
         </is>
       </c>
-      <c r="B77" s="105" t="n">
-        <v>0</v>
+      <c r="B77" s="105">
+        <f>E77+B43-B45</f>
+        <v/>
       </c>
       <c r="C77" s="97">
         <f>B77+C43-C45</f>
@@ -3137,8 +3142,9 @@
           <t>Change in Accounts Receivable</t>
         </is>
       </c>
-      <c r="B90" s="97" t="n">
-        <v>0</v>
+      <c r="B90" s="97">
+        <f>E53-B53</f>
+        <v/>
       </c>
       <c r="C90" s="97">
         <f>B53-C53</f>
@@ -3155,8 +3161,9 @@
           <t>Change in Inventory</t>
         </is>
       </c>
-      <c r="B91" s="97" t="n">
-        <v>0</v>
+      <c r="B91" s="97">
+        <f>E54-B54</f>
+        <v/>
       </c>
       <c r="C91" s="97">
         <f>B54-C54</f>
@@ -3173,8 +3180,9 @@
           <t>Change in Prepaid Expenses</t>
         </is>
       </c>
-      <c r="B92" s="96" t="n">
-        <v>0</v>
+      <c r="B92" s="96">
+        <f>E55-B55</f>
+        <v/>
       </c>
       <c r="C92" s="96">
         <f>B55-C55</f>
@@ -3191,8 +3199,9 @@
           <t>Change in Other Current Assets</t>
         </is>
       </c>
-      <c r="B93" s="96" t="n">
-        <v>0</v>
+      <c r="B93" s="96">
+        <f>E56-B56</f>
+        <v/>
       </c>
       <c r="C93" s="96">
         <f>B56-C56</f>
@@ -3209,8 +3218,9 @@
           <t>Change in Accounts Payable</t>
         </is>
       </c>
-      <c r="B94" s="97" t="n">
-        <v>0</v>
+      <c r="B94" s="97">
+        <f>B66-E66</f>
+        <v/>
       </c>
       <c r="C94" s="97">
         <f>C66-B66</f>
@@ -3227,8 +3237,9 @@
           <t>Change in Accrued Payroll</t>
         </is>
       </c>
-      <c r="B95" s="96" t="n">
-        <v>0</v>
+      <c r="B95" s="96">
+        <f>B67-E67</f>
+        <v/>
       </c>
       <c r="C95" s="96">
         <f>C67-B67</f>
@@ -3245,8 +3256,9 @@
           <t>Change in Deferred Revenue</t>
         </is>
       </c>
-      <c r="B96" s="96" t="n">
-        <v>0</v>
+      <c r="B96" s="96">
+        <f>B68-E68</f>
+        <v/>
       </c>
       <c r="C96" s="96">
         <f>C68-B68</f>
@@ -3263,8 +3275,9 @@
           <t>Change in Interest Payable</t>
         </is>
       </c>
-      <c r="B97" s="96" t="n">
-        <v>0</v>
+      <c r="B97" s="96">
+        <f>B69-E69</f>
+        <v/>
       </c>
       <c r="C97" s="96">
         <f>C69-B69</f>
@@ -3281,8 +3294,9 @@
           <t>Change in Other Current Liabilities</t>
         </is>
       </c>
-      <c r="B98" s="96" t="n">
-        <v>0</v>
+      <c r="B98" s="96">
+        <f>B70-E70</f>
+        <v/>
       </c>
       <c r="C98" s="96">
         <f>C70-B70</f>
@@ -3299,8 +3313,9 @@
           <t>Change in Income Taxes Payable</t>
         </is>
       </c>
-      <c r="B99" s="97" t="n">
-        <v>0</v>
+      <c r="B99" s="97">
+        <f>B71-E71</f>
+        <v/>
       </c>
       <c r="C99" s="97">
         <f>C71-B71</f>
@@ -3352,14 +3367,17 @@
           <t>Acquisitions of Property and Equipment</t>
         </is>
       </c>
-      <c r="B103" s="105" t="n">
-        <v>0</v>
-      </c>
-      <c r="C103" s="105" t="n">
-        <v>0</v>
-      </c>
-      <c r="D103" s="105" t="n">
-        <v>0</v>
+      <c r="B103" s="105">
+        <f>-(B59-E59)</f>
+        <v/>
+      </c>
+      <c r="C103" s="105">
+        <f>-(C59-B59)</f>
+        <v/>
+      </c>
+      <c r="D103" s="105">
+        <f>-(D59-C59)</f>
+        <v/>
       </c>
     </row>
     <row r="104" outlineLevel="1" ht="14.5" customHeight="1">
@@ -3403,8 +3421,9 @@
           <t>Issuance of Common Stock</t>
         </is>
       </c>
-      <c r="B107" s="97" t="n">
-        <v>0</v>
+      <c r="B107" s="97">
+        <f>B76-E76</f>
+        <v/>
       </c>
       <c r="C107" s="97">
         <f>C76-B76</f>
@@ -3440,8 +3459,9 @@
           <t>Increase/(Decrease) in Long-Term Debt</t>
         </is>
       </c>
-      <c r="B109" s="97" t="n">
-        <v>0</v>
+      <c r="B109" s="97">
+        <f>B74-E74</f>
+        <v/>
       </c>
       <c r="C109" s="97">
         <f>C74-B74</f>
@@ -3502,8 +3522,9 @@
           <t>Cash and Equivalents, Beginning of the Year</t>
         </is>
       </c>
-      <c r="B113" s="105" t="n">
-        <v>0</v>
+      <c r="B113" s="105">
+        <f>E52</f>
+        <v/>
       </c>
       <c r="C113" s="97">
         <f>B114</f>
@@ -3702,7 +3723,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>• Best results: Upload a Trial Balance (ending balances) by period/year including Balance Sheet + P&amp;L accounts.</t>
+          <t>Year 0 requirement (internal): Trial Balance must include prior-year year-end snapshot (Year0) for opening balances. Year0 is hidden in the model but used for Year1 cash flow and working capital deltas.</t>
         </is>
       </c>
     </row>
@@ -3720,7 +3741,6 @@
         </is>
       </c>
     </row>
-    <row r="5"/>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
@@ -3735,7 +3755,6 @@
         </is>
       </c>
     </row>
-    <row r="8"/>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>

</xml_diff>